<commit_message>
Fixed some tests. Added some tests for project transfer.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_transfer_v4_10_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_transfer_v4_10_0.xlsx
@@ -2009,7 +2009,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="27.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.21"/>
@@ -2018,15 +2018,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="33.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="30.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="42.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="38.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="38.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="21.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="38.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="34.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="18.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="34.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="61.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="18" style="0" width="9.33"/>
   </cols>
   <sheetData>
@@ -11131,7 +11131,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.33"/>
   </cols>
@@ -12396,7 +12396,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6484375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.5"/>

</xml_diff>